<commit_message>
Backtesting El Dorado and CryptoZen
</commit_message>
<xml_diff>
--- a/Backtesting_PTStratx_search_settings.xlsx
+++ b/Backtesting_PTStratx_search_settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RESULT" sheetId="2" r:id="rId1"/>
@@ -129,12 +129,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C72" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>toytoy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification du captial pour TradingView qui à du mal avec beaucoup d'unité pour par exemple ICX / ONT etc</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="93">
   <si>
     <t>Search Price  Trigger</t>
   </si>
@@ -569,6 +593,126 @@
   <si>
     <t>El_Dorado</t>
   </si>
+  <si>
+    <r>
+      <t>price_rise_trigger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>price_rise_recover_trigger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>price_drop_trigger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>price_drop_recover_trigger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DEFAULT_DCA_buy_percentage_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DEFAULT_DCA_buy_percentage_3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 100</t>
+    </r>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_trigger = -10</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_trigger = -4</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_percentage_1 = 100</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_percentage_2 = 50</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_percentage_4 = 25</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_percentage_5 = 20</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_percentage_3 = 33</t>
+  </si>
+  <si>
+    <t>price_rise_trigger = 7</t>
+  </si>
+  <si>
+    <t>price_rise_recover_trigger = 6</t>
+  </si>
+  <si>
+    <t>price_drop_trigger = 10</t>
+  </si>
+  <si>
+    <t>price_drop_recover_trigger = 3</t>
+  </si>
+  <si>
+    <t>El Dorado 1.0</t>
+  </si>
 </sst>
 </file>
 
@@ -577,7 +721,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +770,24 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -641,7 +803,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -693,11 +855,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,10 +959,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -772,15 +971,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
+  <dxfs count="70">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -813,9 +1095,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -830,6 +1109,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -845,9 +1128,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -879,9 +1159,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -910,6 +1187,45 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -993,106 +1309,127 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A39:K50" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A39:K50" totalsRowShown="0" dataDxfId="69">
   <autoFilter ref="A39:K50"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Name Settings" dataDxfId="55"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="54"/>
-    <tableColumn id="11" name="Captial" dataDxfId="53"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="52"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="51"/>
-    <tableColumn id="2" name="DCA blocked (J)" dataDxfId="50"/>
-    <tableColumn id="5" name="Blocked today " dataDxfId="49"/>
-    <tableColumn id="8" name="Net Profit " dataDxfId="48"/>
-    <tableColumn id="9" name="Closed Trades2" dataDxfId="47"/>
-    <tableColumn id="4" name="DCA blocked (J)2" dataDxfId="46"/>
-    <tableColumn id="10" name="Blocked today" dataDxfId="45"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="68"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="67"/>
+    <tableColumn id="11" name="Captial" dataDxfId="66"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="65"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="64"/>
+    <tableColumn id="2" name="DCA blocked (J)" dataDxfId="63"/>
+    <tableColumn id="5" name="Blocked today " dataDxfId="62"/>
+    <tableColumn id="8" name="Net Profit " dataDxfId="61"/>
+    <tableColumn id="9" name="Closed Trades2" dataDxfId="60"/>
+    <tableColumn id="4" name="DCA blocked (J)2" dataDxfId="59"/>
+    <tableColumn id="10" name="Blocked today" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau25" displayName="Tableau25" ref="A6:L17" totalsRowShown="0" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau25" displayName="Tableau25" ref="A6:L17" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A6:L17"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="43"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="42"/>
-    <tableColumn id="11" name="Captial" dataDxfId="41"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="40"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="39"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="38"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="37"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="36"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="35"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="34"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="33"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="32"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="56"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="55"/>
+    <tableColumn id="11" name="Captial" dataDxfId="54"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="1"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="53"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="52"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="51"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="50"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="49"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="48"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="47"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau257" displayName="Tableau257" ref="A22:L33" totalsRowShown="0" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau257" displayName="Tableau257" ref="A22:L33" totalsRowShown="0" dataDxfId="46">
   <autoFilter ref="A22:L33"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="30"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="29"/>
-    <tableColumn id="11" name="Captial" dataDxfId="28"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="27"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="26"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="25"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="24"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="23"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="22"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="21"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="20"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="19"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="45"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="44"/>
+    <tableColumn id="11" name="Captial" dataDxfId="43"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="2"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="42"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="41"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="40"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="39"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="38"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="37"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="36"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau256" displayName="Tableau256" ref="A56:L67" totalsRowShown="0" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau256" displayName="Tableau256" ref="A56:L67" totalsRowShown="0" dataDxfId="34">
   <autoFilter ref="A56:L67"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="11"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="10"/>
-    <tableColumn id="11" name="Captial" dataDxfId="9"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="8"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="7"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="6"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="5"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="4"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="3"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="2"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="1"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="0"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="33"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="32"/>
+    <tableColumn id="11" name="Captial" dataDxfId="31"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="3"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="30"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="29"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="28"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="27"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="26"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="25"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="24"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C39" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:C39"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="lenght" dataDxfId="16"/>
-    <tableColumn id="2" name="price_drop_trigger" dataDxfId="15"/>
-    <tableColumn id="3" name="ETHBTC - 2h" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau2568" displayName="Tableau2568" ref="A72:L83" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="A72:L83"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Name Settings" dataDxfId="15"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="14"/>
+    <tableColumn id="11" name="Captial" dataDxfId="13"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="4"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="12"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="11"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="10"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="9"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="8"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="7"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="6"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C39" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A2:C39"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="lenght" dataDxfId="21"/>
+    <tableColumn id="2" name="price_drop_trigger" dataDxfId="20"/>
+    <tableColumn id="3" name="ETHBTC - 2h" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="H5:I14" totalsRowShown="0">
   <autoFilter ref="H5:I14"/>
   <tableColumns count="2">
     <tableColumn id="1" name="base 5min"/>
-    <tableColumn id="2" name="candles" dataDxfId="13">
+    <tableColumn id="2" name="candles" dataDxfId="18">
       <calculatedColumnFormula>G6*60/Tableau3[[#This Row],[base 5min]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1363,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1720,7 @@
     <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>53</v>
       </c>
@@ -1397,7 +1734,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>50</v>
       </c>
@@ -1405,7 +1742,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -1413,7 +1750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>64</v>
       </c>
@@ -1429,7 +1766,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1467,7 +1804,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -1477,8 +1814,8 @@
       <c r="C7" s="15">
         <v>2000000</v>
       </c>
-      <c r="D7" s="8">
-        <v>6.6E-3</v>
+      <c r="D7" s="30">
+        <v>0.66</v>
       </c>
       <c r="E7" s="17">
         <v>35</v>
@@ -1501,11 +1838,12 @@
       <c r="K7" s="21">
         <v>22</v>
       </c>
-      <c r="L7" s="24">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="L7" s="30">
+        <v>-5</v>
+      </c>
+      <c r="N7" s="36"/>
+    </row>
+    <row r="8" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>52</v>
       </c>
@@ -1515,8 +1853,8 @@
       <c r="C8" s="15">
         <v>2000000</v>
       </c>
-      <c r="D8" s="8">
-        <v>8.0000000000000004E-4</v>
+      <c r="D8" s="30">
+        <v>0.08</v>
       </c>
       <c r="E8" s="17">
         <v>56</v>
@@ -1539,11 +1877,12 @@
       <c r="K8" s="21">
         <v>10</v>
       </c>
-      <c r="L8" s="24">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="L8" s="30">
+        <v>-5</v>
+      </c>
+      <c r="N8" s="36"/>
+    </row>
+    <row r="9" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>52</v>
       </c>
@@ -1553,8 +1892,8 @@
       <c r="C9" s="15">
         <v>200000</v>
       </c>
-      <c r="D9" s="8">
-        <v>2.0999999999999999E-3</v>
+      <c r="D9" s="30">
+        <v>0.21</v>
       </c>
       <c r="E9" s="17">
         <v>43</v>
@@ -1577,11 +1916,12 @@
       <c r="K9" s="21">
         <v>31</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N9" s="35"/>
+    </row>
+    <row r="10" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>52</v>
       </c>
@@ -1591,8 +1931,8 @@
       <c r="C10" s="15">
         <v>200000</v>
       </c>
-      <c r="D10" s="8">
-        <v>1.06E-2</v>
+      <c r="D10" s="30">
+        <v>1.06</v>
       </c>
       <c r="E10" s="17">
         <v>56</v>
@@ -1615,11 +1955,12 @@
       <c r="K10" s="21">
         <v>5</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>52</v>
       </c>
@@ -1629,8 +1970,8 @@
       <c r="C11" s="15">
         <v>200000</v>
       </c>
-      <c r="D11" s="8">
-        <v>4.8999999999999998E-3</v>
+      <c r="D11" s="30">
+        <v>0.49</v>
       </c>
       <c r="E11" s="17">
         <v>31</v>
@@ -1653,11 +1994,12 @@
       <c r="K11" s="21">
         <v>3</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>52</v>
       </c>
@@ -1667,8 +2009,8 @@
       <c r="C12" s="15">
         <v>200000</v>
       </c>
-      <c r="D12" s="8">
-        <v>7.1999999999999998E-3</v>
+      <c r="D12" s="30">
+        <v>0.72</v>
       </c>
       <c r="E12" s="17">
         <v>23</v>
@@ -1691,11 +2033,12 @@
       <c r="K12" s="21">
         <v>45</v>
       </c>
-      <c r="L12" s="24">
-        <v>-0.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="L12" s="30">
+        <v>-30</v>
+      </c>
+      <c r="N12" s="36"/>
+    </row>
+    <row r="13" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>52</v>
       </c>
@@ -1705,8 +2048,8 @@
       <c r="C13" s="15">
         <v>200000</v>
       </c>
-      <c r="D13" s="8">
-        <v>1.2999999999999999E-3</v>
+      <c r="D13" s="30">
+        <v>0.13</v>
       </c>
       <c r="E13" s="17">
         <v>72</v>
@@ -1729,11 +2072,12 @@
       <c r="K13" s="21">
         <v>4</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N13" s="35"/>
+    </row>
+    <row r="14" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>52</v>
       </c>
@@ -1743,8 +2087,8 @@
       <c r="C14" s="15">
         <v>200000</v>
       </c>
-      <c r="D14" s="8">
-        <v>5.1799999999999999E-2</v>
+      <c r="D14" s="30">
+        <v>5.18</v>
       </c>
       <c r="E14" s="17">
         <v>55</v>
@@ -1767,11 +2111,12 @@
       <c r="K14" s="21">
         <v>3</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N14" s="35"/>
+    </row>
+    <row r="15" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>52</v>
       </c>
@@ -1781,8 +2126,8 @@
       <c r="C15" s="15">
         <v>200000</v>
       </c>
-      <c r="D15" s="8">
-        <v>1.78E-2</v>
+      <c r="D15" s="30">
+        <v>1.78</v>
       </c>
       <c r="E15" s="17">
         <v>64</v>
@@ -1805,11 +2150,12 @@
       <c r="K15" s="21">
         <v>4</v>
       </c>
-      <c r="L15" s="21">
+      <c r="L15" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N15" s="35"/>
+    </row>
+    <row r="16" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>52</v>
       </c>
@@ -1819,8 +2165,8 @@
       <c r="C16" s="15">
         <v>20000</v>
       </c>
-      <c r="D16" s="8">
-        <v>6.7999999999999996E-3</v>
+      <c r="D16" s="30">
+        <v>0.68</v>
       </c>
       <c r="E16" s="17">
         <v>42</v>
@@ -1843,11 +2189,12 @@
       <c r="K16" s="21">
         <v>15</v>
       </c>
-      <c r="L16" s="24">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="L16" s="30">
+        <v>0</v>
+      </c>
+      <c r="N16" s="36"/>
+    </row>
+    <row r="17" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>52</v>
       </c>
@@ -1857,8 +2204,8 @@
       <c r="C17" s="15">
         <v>20000</v>
       </c>
-      <c r="D17" s="8">
-        <v>4.0000000000000001E-3</v>
+      <c r="D17" s="30">
+        <v>0.4</v>
       </c>
       <c r="E17" s="17">
         <v>21</v>
@@ -1881,11 +2228,12 @@
       <c r="K17" s="22">
         <v>22</v>
       </c>
-      <c r="L17" s="25">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="31">
+        <v>-20</v>
+      </c>
+      <c r="N17" s="36"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="15"/>
@@ -1894,50 +2242,50 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="38">
         <f>AVERAGE(Tableau25[Net Profit (%)])</f>
-        <v>1.0354545454545455E-2</v>
-      </c>
-      <c r="E19" s="26">
+        <v>1.0354545454545454</v>
+      </c>
+      <c r="E19" s="39">
         <f>AVERAGE(Tableau25[Closed Trades])</f>
         <v>45.272727272727273</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="39">
         <f>AVERAGE(Tableau25[% Profitable])</f>
         <v>50.899090909090908</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="39">
         <f>AVERAGE(Tableau25[Profit Factor])</f>
         <v>1.922181818181818</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="39">
         <f>AVERAGE(Tableau25[Max DrawDown])</f>
         <v>1.1969999999999998</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="39">
         <f>AVERAGE(Tableau25[Avg Trade])</f>
         <v>2.2727272727272724E-2</v>
       </c>
-      <c r="J19" s="26">
+      <c r="J19" s="39">
         <f>AVERAGE(Tableau25[Avg Bars in Trade])</f>
         <v>13.182727272727272</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="39">
         <f>AVERAGE(Tableau25[DCA blocked (J)])</f>
         <v>14.909090909090908</v>
       </c>
-      <c r="L19" s="26">
+      <c r="L19" s="40">
         <f>AVERAGE(Tableau25[[Blocked today ]])</f>
-        <v>-5.909090909090909E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-5.4545454545454541</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>63</v>
       </c>
@@ -1953,7 +2301,7 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>12</v>
       </c>
@@ -1991,7 +2339,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>63</v>
       </c>
@@ -2001,35 +2349,17 @@
       <c r="C23" s="15">
         <v>2000000</v>
       </c>
-      <c r="D23" s="8">
-        <v>6.6E-3</v>
-      </c>
-      <c r="E23" s="17">
-        <v>35</v>
-      </c>
-      <c r="F23" s="17">
-        <v>36.11</v>
-      </c>
-      <c r="G23" s="17">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H23" s="17">
-        <v>0.93</v>
-      </c>
-      <c r="I23" s="17">
-        <v>0.02</v>
-      </c>
-      <c r="J23" s="17">
-        <v>32</v>
-      </c>
-      <c r="K23" s="21">
-        <v>22</v>
-      </c>
-      <c r="L23" s="24">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="8"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>63</v>
       </c>
@@ -2039,35 +2369,17 @@
       <c r="C24" s="15">
         <v>2000000</v>
       </c>
-      <c r="D24" s="8">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="E24" s="17">
-        <v>56</v>
-      </c>
-      <c r="F24" s="17">
-        <v>46.03</v>
-      </c>
-      <c r="G24" s="17">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="H24" s="17">
-        <v>1.7769999999999999</v>
-      </c>
-      <c r="I24" s="17">
-        <v>0.01</v>
-      </c>
-      <c r="J24" s="17">
-        <v>0.01</v>
-      </c>
-      <c r="K24" s="21">
-        <v>10</v>
-      </c>
-      <c r="L24" s="24">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="8"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>63</v>
       </c>
@@ -2077,35 +2389,17 @@
       <c r="C25" s="15">
         <v>200000</v>
       </c>
-      <c r="D25" s="8">
-        <v>2.0999999999999999E-3</v>
-      </c>
-      <c r="E25" s="17">
-        <v>43</v>
-      </c>
-      <c r="F25" s="17">
-        <v>50</v>
-      </c>
-      <c r="G25" s="17">
-        <v>1.111</v>
-      </c>
-      <c r="H25" s="17">
-        <v>0.99</v>
-      </c>
-      <c r="I25" s="17">
-        <v>0</v>
-      </c>
-      <c r="J25" s="17">
-        <v>48</v>
-      </c>
-      <c r="K25" s="21">
-        <v>31</v>
-      </c>
-      <c r="L25" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="8"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+    </row>
+    <row r="26" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>63</v>
       </c>
@@ -2115,35 +2409,17 @@
       <c r="C26" s="15">
         <v>200000</v>
       </c>
-      <c r="D26" s="8">
-        <v>1.06E-2</v>
-      </c>
-      <c r="E26" s="17">
-        <v>56</v>
-      </c>
-      <c r="F26" s="17">
-        <v>52.86</v>
-      </c>
-      <c r="G26" s="17">
-        <v>1.764</v>
-      </c>
-      <c r="H26" s="17">
-        <v>0.95</v>
-      </c>
-      <c r="I26" s="17">
-        <v>0.02</v>
-      </c>
-      <c r="J26" s="17">
-        <v>12</v>
-      </c>
-      <c r="K26" s="21">
-        <v>5</v>
-      </c>
-      <c r="L26" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="8"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+    </row>
+    <row r="27" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>63</v>
       </c>
@@ -2153,35 +2429,17 @@
       <c r="C27" s="15">
         <v>200000</v>
       </c>
-      <c r="D27" s="8">
-        <v>4.8999999999999998E-3</v>
-      </c>
-      <c r="E27" s="17">
-        <v>31</v>
-      </c>
-      <c r="F27" s="17">
-        <v>52.94</v>
-      </c>
-      <c r="G27" s="17">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="H27" s="17">
-        <v>1.68</v>
-      </c>
-      <c r="I27" s="17">
-        <v>0.01</v>
-      </c>
-      <c r="J27" s="17">
-        <v>7</v>
-      </c>
-      <c r="K27" s="21">
-        <v>3</v>
-      </c>
-      <c r="L27" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="8"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+    </row>
+    <row r="28" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>63</v>
       </c>
@@ -2191,35 +2449,17 @@
       <c r="C28" s="15">
         <v>200000</v>
       </c>
-      <c r="D28" s="8">
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="E28" s="17">
-        <v>23</v>
-      </c>
-      <c r="F28" s="17">
-        <v>65.38</v>
-      </c>
-      <c r="G28" s="17">
-        <v>3.97</v>
-      </c>
-      <c r="H28" s="17">
-        <v>0.21</v>
-      </c>
-      <c r="I28" s="17">
-        <v>0.03</v>
-      </c>
-      <c r="J28" s="17">
-        <v>4</v>
-      </c>
-      <c r="K28" s="21">
-        <v>45</v>
-      </c>
-      <c r="L28" s="24">
-        <v>-0.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="8"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="24"/>
+    </row>
+    <row r="29" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>63</v>
       </c>
@@ -2229,35 +2469,17 @@
       <c r="C29" s="15">
         <v>200000</v>
       </c>
-      <c r="D29" s="8">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="E29" s="17">
-        <v>72</v>
-      </c>
-      <c r="F29" s="17">
-        <v>51.17</v>
-      </c>
-      <c r="G29" s="17">
-        <v>1.08</v>
-      </c>
-      <c r="H29" s="17">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I29" s="17">
-        <v>0</v>
-      </c>
-      <c r="J29" s="17">
-        <v>10</v>
-      </c>
-      <c r="K29" s="21">
-        <v>4</v>
-      </c>
-      <c r="L29" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+    </row>
+    <row r="30" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>63</v>
       </c>
@@ -2267,35 +2489,17 @@
       <c r="C30" s="15">
         <v>200000</v>
       </c>
-      <c r="D30" s="8">
-        <v>5.1799999999999999E-2</v>
-      </c>
-      <c r="E30" s="17">
-        <v>55</v>
-      </c>
-      <c r="F30" s="17">
-        <v>36.36</v>
-      </c>
-      <c r="G30" s="17">
-        <v>9.4E-2</v>
-      </c>
-      <c r="H30" s="17">
-        <v>5.37</v>
-      </c>
-      <c r="I30" s="17">
-        <v>0.09</v>
-      </c>
-      <c r="J30" s="17">
-        <v>6</v>
-      </c>
-      <c r="K30" s="21">
-        <v>3</v>
-      </c>
-      <c r="L30" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="8"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+    </row>
+    <row r="31" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>63</v>
       </c>
@@ -2305,35 +2509,17 @@
       <c r="C31" s="15">
         <v>200000</v>
       </c>
-      <c r="D31" s="8">
-        <v>1.78E-2</v>
-      </c>
-      <c r="E31" s="17">
-        <v>64</v>
-      </c>
-      <c r="F31" s="17">
-        <v>50</v>
-      </c>
-      <c r="G31" s="17">
-        <v>2.0880000000000001</v>
-      </c>
-      <c r="H31" s="17">
-        <v>0.47</v>
-      </c>
-      <c r="I31" s="17">
-        <v>0.03</v>
-      </c>
-      <c r="J31" s="17">
-        <v>16</v>
-      </c>
-      <c r="K31" s="21">
-        <v>4</v>
-      </c>
-      <c r="L31" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+    </row>
+    <row r="32" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>63</v>
       </c>
@@ -2343,35 +2529,17 @@
       <c r="C32" s="15">
         <v>20000</v>
       </c>
-      <c r="D32" s="8">
-        <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="E32" s="17">
-        <v>42</v>
-      </c>
-      <c r="F32" s="17">
-        <v>57.14</v>
-      </c>
-      <c r="G32" s="17">
-        <v>2.048</v>
-      </c>
-      <c r="H32" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="I32" s="17">
-        <v>0.02</v>
-      </c>
-      <c r="J32" s="17">
-        <v>6</v>
-      </c>
-      <c r="K32" s="21">
-        <v>15</v>
-      </c>
-      <c r="L32" s="24">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="24"/>
+    </row>
+    <row r="33" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>63</v>
       </c>
@@ -2381,35 +2549,17 @@
       <c r="C33" s="15">
         <v>20000</v>
       </c>
-      <c r="D33" s="8">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E33" s="17">
-        <v>21</v>
-      </c>
-      <c r="F33" s="17">
-        <v>61.9</v>
-      </c>
-      <c r="G33" s="17">
-        <v>6.8</v>
-      </c>
-      <c r="H33" s="17">
-        <v>0.03</v>
-      </c>
-      <c r="I33" s="17">
-        <v>0.02</v>
-      </c>
-      <c r="J33" s="17">
-        <v>4</v>
-      </c>
-      <c r="K33" s="22">
-        <v>22</v>
-      </c>
-      <c r="L33" s="25">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D33" s="8"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="25"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
       <c r="C34" s="15"/>
@@ -2418,48 +2568,21 @@
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="27">
-        <f>AVERAGE(Tableau257[Net Profit (%)])</f>
-        <v>1.0354545454545455E-2</v>
-      </c>
-      <c r="E35" s="26">
-        <f>AVERAGE(Tableau257[Closed Trades])</f>
-        <v>45.272727272727273</v>
-      </c>
-      <c r="F35" s="26">
-        <f>AVERAGE(Tableau257[% Profitable])</f>
-        <v>50.899090909090908</v>
-      </c>
-      <c r="G35" s="26">
-        <f>AVERAGE(Tableau257[Profit Factor])</f>
-        <v>1.922181818181818</v>
-      </c>
-      <c r="H35" s="26">
-        <f>AVERAGE(Tableau257[Max DrawDown])</f>
-        <v>1.1969999999999998</v>
-      </c>
-      <c r="I35" s="26">
-        <f>AVERAGE(Tableau257[Avg Trade])</f>
-        <v>2.2727272727272724E-2</v>
-      </c>
-      <c r="J35" s="26">
-        <f>AVERAGE(Tableau257[Avg Bars in Trade])</f>
-        <v>13.182727272727272</v>
-      </c>
-      <c r="K35" s="26">
-        <f>AVERAGE(Tableau257[DCA blocked (J)])</f>
-        <v>14.909090909090908</v>
-      </c>
-      <c r="L35" s="26">
-        <f>AVERAGE(Tableau257[[Blocked today ]])</f>
-        <v>-5.909090909090909E-2</v>
-      </c>
+      <c r="D35" s="38"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="40"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H36" s="13"/>
@@ -2851,7 +2974,7 @@
         <v>-0.23</v>
       </c>
     </row>
-    <row r="51" spans="1:12" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="C51" s="15"/>
       <c r="D51" s="8"/>
@@ -2861,34 +2984,34 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
-      <c r="C52" s="30" t="s">
+      <c r="C52" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="42">
         <f>AVERAGE(Tableau2[Net Profit (%)])</f>
         <v>2.4087499999999998E-2</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="43">
         <f>AVERAGE(Tableau2[Closed Trades])</f>
         <v>62.125</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="7">
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43">
         <f>AVERAGE(Tableau2[[Net Profit ]])</f>
         <v>4.4745454545454555</v>
       </c>
-      <c r="I52" s="7">
+      <c r="I52" s="43">
         <f>AVERAGE(Tableau2[Closed Trades2])</f>
         <v>120.72727272727273</v>
       </c>
-      <c r="J52" s="13">
+      <c r="J52" s="43">
         <f>AVERAGE(Tableau2[DCA blocked (J)2])</f>
         <v>67.818181818181813</v>
       </c>
-      <c r="K52" s="13">
+      <c r="K52" s="44">
         <f>AVERAGE(Tableau2[Blocked today])</f>
         <v>-0.17181818181818184</v>
       </c>
@@ -2966,32 +3089,32 @@
       <c r="C57" s="15">
         <v>2000000</v>
       </c>
-      <c r="D57" s="8">
-        <v>6.6E-3</v>
+      <c r="D57" s="30">
+        <v>2.88</v>
       </c>
       <c r="E57" s="20">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="F57" s="20">
-        <v>36.11</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="G57" s="20">
-        <v>0.57999999999999996</v>
+        <v>2.948</v>
       </c>
       <c r="H57" s="20">
-        <v>0.93</v>
+        <v>0.75</v>
       </c>
       <c r="I57" s="20">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J57" s="20">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K57" s="21">
-        <v>22</v>
-      </c>
-      <c r="L57" s="24">
-        <v>-0.05</v>
+        <v>120</v>
+      </c>
+      <c r="L57" s="30">
+        <v>-32</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3004,32 +3127,32 @@
       <c r="C58" s="15">
         <v>2000000</v>
       </c>
-      <c r="D58" s="8">
-        <v>8.0000000000000004E-4</v>
+      <c r="D58" s="30">
+        <v>2.89</v>
       </c>
       <c r="E58" s="20">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F58" s="20">
-        <v>46.03</v>
+        <v>85.14</v>
       </c>
       <c r="G58" s="20">
-        <v>0.78500000000000003</v>
+        <v>2.145</v>
       </c>
       <c r="H58" s="20">
-        <v>1.7769999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="I58" s="20">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="J58" s="20">
-        <v>0.01</v>
+        <v>136</v>
       </c>
       <c r="K58" s="21">
-        <v>10</v>
-      </c>
-      <c r="L58" s="24">
-        <v>-0.05</v>
+        <v>54</v>
+      </c>
+      <c r="L58" s="30">
+        <v>-8</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3042,32 +3165,32 @@
       <c r="C59" s="15">
         <v>200000</v>
       </c>
-      <c r="D59" s="8">
-        <v>2.0999999999999999E-3</v>
+      <c r="D59" s="30">
+        <v>5.33</v>
       </c>
       <c r="E59" s="20">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="F59" s="20">
-        <v>50</v>
+        <v>82.09</v>
       </c>
       <c r="G59" s="20">
-        <v>1.111</v>
+        <v>7.4240000000000004</v>
       </c>
       <c r="H59" s="20">
-        <v>0.99</v>
+        <v>0.35</v>
       </c>
       <c r="I59" s="20">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J59" s="20">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="K59" s="21">
-        <v>31</v>
-      </c>
-      <c r="L59" s="21">
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="L59" s="30">
+        <v>-7</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -3080,32 +3203,32 @@
       <c r="C60" s="15">
         <v>200000</v>
       </c>
-      <c r="D60" s="8">
-        <v>1.06E-2</v>
+      <c r="D60" s="30">
+        <v>2.62</v>
       </c>
       <c r="E60" s="20">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="F60" s="20">
-        <v>52.86</v>
+        <v>81.48</v>
       </c>
       <c r="G60" s="20">
-        <v>1.764</v>
+        <v>5.7089999999999996</v>
       </c>
       <c r="H60" s="20">
-        <v>0.95</v>
+        <v>0.54</v>
       </c>
       <c r="I60" s="20">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="J60" s="20">
-        <v>12</v>
+        <v>415</v>
       </c>
       <c r="K60" s="21">
-        <v>5</v>
-      </c>
-      <c r="L60" s="21">
-        <v>0</v>
+        <v>125</v>
+      </c>
+      <c r="L60" s="30">
+        <v>-30</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3118,32 +3241,32 @@
       <c r="C61" s="15">
         <v>200000</v>
       </c>
-      <c r="D61" s="8">
-        <v>4.8999999999999998E-3</v>
+      <c r="D61" s="30">
+        <v>2.48</v>
       </c>
       <c r="E61" s="20">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F61" s="20">
-        <v>52.94</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="G61" s="20">
-        <v>0.82399999999999995</v>
+        <v>4.4279999999999999</v>
       </c>
       <c r="H61" s="20">
-        <v>1.68</v>
+        <v>0.41</v>
       </c>
       <c r="I61" s="20">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="J61" s="20">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="K61" s="21">
-        <v>3</v>
-      </c>
-      <c r="L61" s="21">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="L61" s="30">
+        <v>-22</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -3156,32 +3279,32 @@
       <c r="C62" s="15">
         <v>200000</v>
       </c>
-      <c r="D62" s="8">
-        <v>7.1999999999999998E-3</v>
+      <c r="D62" s="30">
+        <v>2.5</v>
       </c>
       <c r="E62" s="20">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F62" s="20">
-        <v>65.38</v>
+        <v>77.78</v>
       </c>
       <c r="G62" s="20">
-        <v>3.97</v>
+        <v>5.6280000000000001</v>
       </c>
       <c r="H62" s="20">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="I62" s="20">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J62" s="20">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="K62" s="21">
-        <v>45</v>
-      </c>
-      <c r="L62" s="24">
-        <v>-0.3</v>
+        <v>66</v>
+      </c>
+      <c r="L62" s="30">
+        <v>-37</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3194,32 +3317,32 @@
       <c r="C63" s="15">
         <v>200000</v>
       </c>
-      <c r="D63" s="8">
-        <v>1.2999999999999999E-3</v>
+      <c r="D63" s="30">
+        <v>3.41</v>
       </c>
       <c r="E63" s="20">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F63" s="20">
-        <v>51.17</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="G63" s="20">
-        <v>1.08</v>
+        <v>1.89</v>
       </c>
       <c r="H63" s="20">
-        <v>0.56000000000000005</v>
+        <v>1.52</v>
       </c>
       <c r="I63" s="20">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J63" s="20">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="K63" s="21">
-        <v>4</v>
-      </c>
-      <c r="L63" s="21">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="L63" s="30">
+        <v>-5</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -3232,32 +3355,32 @@
       <c r="C64" s="15">
         <v>200000</v>
       </c>
-      <c r="D64" s="8">
-        <v>5.1799999999999999E-2</v>
+      <c r="D64" s="30">
+        <v>2.36</v>
       </c>
       <c r="E64" s="20">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F64" s="20">
-        <v>36.36</v>
+        <v>80.430000000000007</v>
       </c>
       <c r="G64" s="20">
-        <v>9.4E-2</v>
+        <v>3.0950000000000002</v>
       </c>
       <c r="H64" s="20">
-        <v>5.37</v>
+        <v>0.34</v>
       </c>
       <c r="I64" s="20">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="J64" s="20">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="K64" s="21">
-        <v>3</v>
-      </c>
-      <c r="L64" s="21">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="L64" s="30">
+        <v>-4</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3270,32 +3393,32 @@
       <c r="C65" s="15">
         <v>200000</v>
       </c>
-      <c r="D65" s="8">
-        <v>1.78E-2</v>
+      <c r="D65" s="30">
+        <v>1.59</v>
       </c>
       <c r="E65" s="20">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F65" s="20">
-        <v>50</v>
+        <v>72.73</v>
       </c>
       <c r="G65" s="20">
-        <v>2.0880000000000001</v>
+        <v>14.968</v>
       </c>
       <c r="H65" s="20">
-        <v>0.47</v>
+        <v>0.11</v>
       </c>
       <c r="I65" s="20">
-        <v>0.03</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J65" s="20">
         <v>16</v>
       </c>
       <c r="K65" s="21">
-        <v>4</v>
-      </c>
-      <c r="L65" s="21">
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="L65" s="30">
+        <v>-50</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3308,32 +3431,32 @@
       <c r="C66" s="15">
         <v>20000</v>
       </c>
-      <c r="D66" s="8">
-        <v>6.7999999999999996E-3</v>
+      <c r="D66" s="30">
+        <v>4.01</v>
       </c>
       <c r="E66" s="20">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F66" s="20">
-        <v>57.14</v>
+        <v>78.05</v>
       </c>
       <c r="G66" s="20">
-        <v>2.048</v>
+        <v>3.6389999999999998</v>
       </c>
       <c r="H66" s="20">
-        <v>0.2</v>
+        <v>0.65</v>
       </c>
       <c r="I66" s="20">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="J66" s="20">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="K66" s="21">
-        <v>15</v>
-      </c>
-      <c r="L66" s="24">
-        <v>-0.05</v>
+        <v>73</v>
+      </c>
+      <c r="L66" s="30">
+        <v>-16</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3346,35 +3469,35 @@
       <c r="C67" s="15">
         <v>20000</v>
       </c>
-      <c r="D67" s="8">
-        <v>4.0000000000000001E-3</v>
+      <c r="D67" s="30">
+        <v>1.77</v>
       </c>
       <c r="E67" s="20">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F67" s="20">
-        <v>61.9</v>
+        <v>80.56</v>
       </c>
       <c r="G67" s="20">
-        <v>6.8</v>
+        <v>3.7719999999999998</v>
       </c>
       <c r="H67" s="20">
-        <v>0.03</v>
+        <v>0.41</v>
       </c>
       <c r="I67" s="20">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="J67" s="20">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="K67" s="22">
-        <v>22</v>
-      </c>
-      <c r="L67" s="25">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="L67" s="31">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
       <c r="B68" s="20"/>
       <c r="C68" s="15"/>
@@ -3383,52 +3506,577 @@
       <c r="F68" s="20"/>
       <c r="G68" s="20"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="20"/>
-      <c r="C69" s="26" t="s">
+      <c r="C69" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D69" s="27">
+      <c r="D69" s="38">
         <f>AVERAGE(Tableau256[Net Profit (%)])</f>
-        <v>1.0354545454545455E-2</v>
-      </c>
-      <c r="E69" s="26">
+        <v>2.8945454545454545</v>
+      </c>
+      <c r="E69" s="39">
         <f>AVERAGE(Tableau256[Closed Trades])</f>
-        <v>45.272727272727273</v>
-      </c>
-      <c r="F69" s="26">
+        <v>48.454545454545453</v>
+      </c>
+      <c r="F69" s="39">
         <f>AVERAGE(Tableau256[% Profitable])</f>
-        <v>50.899090909090908</v>
-      </c>
-      <c r="G69" s="26">
+        <v>79.979090909090914</v>
+      </c>
+      <c r="G69" s="39">
         <f>AVERAGE(Tableau256[Profit Factor])</f>
-        <v>1.922181818181818</v>
-      </c>
-      <c r="H69" s="26">
+        <v>5.058727272727273</v>
+      </c>
+      <c r="H69" s="39">
         <f>AVERAGE(Tableau256[Max DrawDown])</f>
-        <v>1.1969999999999998</v>
-      </c>
-      <c r="I69" s="26">
+        <v>0.56363636363636371</v>
+      </c>
+      <c r="I69" s="39">
         <f>AVERAGE(Tableau256[Avg Trade])</f>
-        <v>2.2727272727272724E-2</v>
-      </c>
-      <c r="J69" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J69" s="39">
         <f>AVERAGE(Tableau256[Avg Bars in Trade])</f>
-        <v>13.182727272727272</v>
-      </c>
-      <c r="K69" s="26">
+        <v>88.63636363636364</v>
+      </c>
+      <c r="K69" s="39">
         <f>AVERAGE(Tableau256[DCA blocked (J)])</f>
-        <v>14.909090909090908</v>
-      </c>
-      <c r="L69" s="26">
+        <v>81.818181818181813</v>
+      </c>
+      <c r="L69" s="40">
         <f>AVERAGE(Tableau256[[Blocked today ]])</f>
-        <v>-5.909090909090909E-2</v>
+        <v>-20.09090909090909</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G72" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H72" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I72" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J72" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="K72" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="L72" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="15">
+        <v>2000000</v>
+      </c>
+      <c r="D73" s="30">
+        <v>16.48</v>
+      </c>
+      <c r="E73" s="27">
+        <v>137</v>
+      </c>
+      <c r="F73" s="27">
+        <v>8394</v>
+      </c>
+      <c r="G73" s="27">
+        <v>5.3140000000000001</v>
+      </c>
+      <c r="H73" s="27">
+        <v>0.85</v>
+      </c>
+      <c r="I73" s="27">
+        <v>0.12</v>
+      </c>
+      <c r="J73" s="27">
+        <v>25</v>
+      </c>
+      <c r="K73" s="21">
+        <v>53</v>
+      </c>
+      <c r="L73" s="30">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="15">
+        <v>2000000</v>
+      </c>
+      <c r="D74" s="30">
+        <v>55.57</v>
+      </c>
+      <c r="E74" s="27">
+        <v>107</v>
+      </c>
+      <c r="F74" s="27">
+        <v>78.5</v>
+      </c>
+      <c r="G74" s="27">
+        <v>5.016</v>
+      </c>
+      <c r="H74" s="27">
+        <v>7.74</v>
+      </c>
+      <c r="I74" s="27">
+        <v>0.52</v>
+      </c>
+      <c r="J74" s="27">
+        <v>55</v>
+      </c>
+      <c r="K74" s="21">
+        <v>30</v>
+      </c>
+      <c r="L74" s="30">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D75" s="30">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="E75" s="27">
+        <v>112</v>
+      </c>
+      <c r="F75" s="27">
+        <v>7321</v>
+      </c>
+      <c r="G75" s="27">
+        <v>3.3260000000000001</v>
+      </c>
+      <c r="H75" s="27">
+        <v>5.45</v>
+      </c>
+      <c r="I75" s="27">
+        <v>0.18</v>
+      </c>
+      <c r="J75" s="27">
+        <v>66</v>
+      </c>
+      <c r="K75" s="21">
+        <v>23</v>
+      </c>
+      <c r="L75" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D76" s="30">
+        <v>10.66</v>
+      </c>
+      <c r="E76" s="27">
+        <v>93</v>
+      </c>
+      <c r="F76" s="27">
+        <v>63.44</v>
+      </c>
+      <c r="G76" s="27">
+        <v>2.024</v>
+      </c>
+      <c r="H76" s="27">
+        <v>5.24</v>
+      </c>
+      <c r="I76" s="27">
+        <v>0.11</v>
+      </c>
+      <c r="J76" s="27">
+        <v>60</v>
+      </c>
+      <c r="K76" s="21">
+        <v>47</v>
+      </c>
+      <c r="L76" s="30">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D77" s="30">
+        <v>3.81</v>
+      </c>
+      <c r="E77" s="27">
+        <v>55</v>
+      </c>
+      <c r="F77" s="27">
+        <v>78.180000000000007</v>
+      </c>
+      <c r="G77" s="27">
+        <v>4.9690000000000003</v>
+      </c>
+      <c r="H77" s="27">
+        <v>0.43</v>
+      </c>
+      <c r="I77" s="27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J77" s="27">
+        <v>16</v>
+      </c>
+      <c r="K77" s="21">
+        <v>25</v>
+      </c>
+      <c r="L77" s="30">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D78" s="30">
+        <v>7.25</v>
+      </c>
+      <c r="E78" s="27">
+        <v>81</v>
+      </c>
+      <c r="F78" s="27">
+        <v>63.74</v>
+      </c>
+      <c r="G78" s="27">
+        <v>2.1230000000000002</v>
+      </c>
+      <c r="H78" s="27">
+        <v>1.54</v>
+      </c>
+      <c r="I78" s="27">
+        <v>0.08</v>
+      </c>
+      <c r="J78" s="27">
+        <v>39</v>
+      </c>
+      <c r="K78" s="21">
+        <v>16</v>
+      </c>
+      <c r="L78" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D79" s="30">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="E79" s="27">
+        <v>126</v>
+      </c>
+      <c r="F79" s="27">
+        <v>73.81</v>
+      </c>
+      <c r="G79" s="27">
+        <v>2.9380000000000002</v>
+      </c>
+      <c r="H79" s="27">
+        <v>2.9380000000000002</v>
+      </c>
+      <c r="I79" s="27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J79" s="27">
+        <v>39</v>
+      </c>
+      <c r="K79" s="21">
+        <v>29</v>
+      </c>
+      <c r="L79" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D80" s="30">
+        <v>11.11</v>
+      </c>
+      <c r="E80" s="27">
+        <v>110</v>
+      </c>
+      <c r="F80" s="27">
+        <v>73.64</v>
+      </c>
+      <c r="G80" s="27">
+        <v>2.64</v>
+      </c>
+      <c r="H80" s="27">
+        <v>3.36</v>
+      </c>
+      <c r="I80" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="J80" s="27">
+        <v>47</v>
+      </c>
+      <c r="K80" s="21">
+        <v>51</v>
+      </c>
+      <c r="L80" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D81" s="30">
+        <v>10.66</v>
+      </c>
+      <c r="E81" s="27">
+        <v>87</v>
+      </c>
+      <c r="F81" s="27">
+        <v>72.41</v>
+      </c>
+      <c r="G81" s="27">
+        <v>3.19</v>
+      </c>
+      <c r="H81" s="27">
+        <v>3.19</v>
+      </c>
+      <c r="I81" s="27">
+        <v>0.12</v>
+      </c>
+      <c r="J81" s="27">
+        <v>41</v>
+      </c>
+      <c r="K81" s="21">
+        <v>25</v>
+      </c>
+      <c r="L81" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C82" s="15">
+        <v>20000</v>
+      </c>
+      <c r="D82" s="30">
+        <v>5.57</v>
+      </c>
+      <c r="E82" s="27">
+        <v>88</v>
+      </c>
+      <c r="F82" s="27">
+        <v>63.64</v>
+      </c>
+      <c r="G82" s="27">
+        <v>1.97</v>
+      </c>
+      <c r="H82" s="27">
+        <v>1.79</v>
+      </c>
+      <c r="I82" s="27">
+        <v>0.06</v>
+      </c>
+      <c r="J82" s="27">
+        <v>49</v>
+      </c>
+      <c r="K82" s="21">
+        <v>26</v>
+      </c>
+      <c r="L82" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="15">
+        <v>20000</v>
+      </c>
+      <c r="D83" s="30">
+        <v>4.59</v>
+      </c>
+      <c r="E83" s="27">
+        <v>61</v>
+      </c>
+      <c r="F83" s="27">
+        <v>67.209999999999994</v>
+      </c>
+      <c r="G83" s="27">
+        <v>1.4770000000000001</v>
+      </c>
+      <c r="H83" s="27">
+        <v>8</v>
+      </c>
+      <c r="I83" s="27">
+        <v>0.08</v>
+      </c>
+      <c r="J83" s="27">
+        <v>50</v>
+      </c>
+      <c r="K83" s="22">
+        <v>25</v>
+      </c>
+      <c r="L83" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="27"/>
+    </row>
+    <row r="85" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="38">
+        <f>AVERAGE(Tableau2568[Net Profit (%)])</f>
+        <v>14.811818181818182</v>
+      </c>
+      <c r="E85" s="39">
+        <f>AVERAGE(Tableau2568[Closed Trades])</f>
+        <v>96.090909090909093</v>
+      </c>
+      <c r="F85" s="39">
+        <f>AVERAGE(Tableau2568[% Profitable])</f>
+        <v>1486.3245454545452</v>
+      </c>
+      <c r="G85" s="39">
+        <f>AVERAGE(Tableau2568[Profit Factor])</f>
+        <v>3.1806363636363639</v>
+      </c>
+      <c r="H85" s="39">
+        <f>AVERAGE(Tableau2568[Max DrawDown])</f>
+        <v>3.6843636363636363</v>
+      </c>
+      <c r="I85" s="39">
+        <f>AVERAGE(Tableau2568[Avg Trade])</f>
+        <v>0.14363636363636367</v>
+      </c>
+      <c r="J85" s="39">
+        <f>AVERAGE(Tableau2568[Avg Bars in Trade])</f>
+        <v>44.272727272727273</v>
+      </c>
+      <c r="K85" s="39">
+        <f>AVERAGE(Tableau2568[DCA blocked (J)])</f>
+        <v>31.818181818181817</v>
+      </c>
+      <c r="L85" s="40">
+        <f>AVERAGE(Tableau2568[[Blocked today ]])</f>
+        <v>-3.0909090909090908</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A71:L71"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="H38:K38"/>
     <mergeCell ref="A5:L5"/>
@@ -3436,7 +4084,7 @@
     <mergeCell ref="A55:L55"/>
   </mergeCells>
   <conditionalFormatting sqref="D39:E39 D38 E40:G50 G39">
-    <cfRule type="dataBar" priority="59">
+    <cfRule type="dataBar" priority="78">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3450,7 +4098,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D50">
-    <cfRule type="dataBar" priority="62">
+    <cfRule type="dataBar" priority="81">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3463,8 +4111,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:I51 J40:K50 I20 K39 I53:I54 I70:I1048576">
-    <cfRule type="dataBar" priority="30">
+  <conditionalFormatting sqref="I39:I51 J40:K50 I20 K39 I53:I54 I70 I86:I1048576">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3478,7 +4126,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D17">
-    <cfRule type="dataBar" priority="28">
+    <cfRule type="dataBar" priority="47">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3492,7 +4140,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:K37">
-    <cfRule type="dataBar" priority="26">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3506,7 +4154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="dataBar" priority="29">
+    <cfRule type="dataBar" priority="48">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3520,7 +4168,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:L7">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3534,7 +4182,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="43">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3548,7 +4196,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3561,8 +4209,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:H51 H20 H53:H54 H70:H1048576">
-    <cfRule type="dataBar" priority="72">
+  <conditionalFormatting sqref="H38:H51 H20 H53:H54 H70 H86:H1048576">
+    <cfRule type="dataBar" priority="91">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3576,7 +4224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L6 D6:E6 K8:L17 E7:E17">
-    <cfRule type="dataBar" priority="73">
+    <cfRule type="dataBar" priority="92">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3590,7 +4238,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F17">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3604,7 +4252,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G17">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3618,7 +4266,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H17">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3632,7 +4280,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I17">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3646,7 +4294,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J17">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3659,22 +4307,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23:D33">
-    <cfRule type="dataBar" priority="15">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{476397F3-E88D-4891-9A86-1454E9281DAC}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K23:L23">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3688,7 +4322,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:L22 D22:E22 K24:L33 E23:E33">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3702,7 +4336,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F33">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3716,7 +4350,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:G33">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3730,7 +4364,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H33">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3744,7 +4378,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I33">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3758,7 +4392,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J33">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3771,22 +4405,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57:D67">
-    <cfRule type="dataBar" priority="7">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{42F8FBF0-D54C-4CD6-9F3F-B8267C763866}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K57:L57">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="K57">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3799,8 +4419,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K56:L56 D56:E56 K58:L67 E57:E67">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="K56:L56 D56:E56 K59:L59 E57:E67 K58 K66:L67 K60:K65">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3814,7 +4434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F67">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3828,7 +4448,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:G67">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3842,7 +4462,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56:H67">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3856,7 +4476,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:I67">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3870,7 +4490,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:J67">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3883,14 +4503,281 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L57:L58">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CCF4670A-9CCA-4C1C-967F-45C4C21C6884}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L60:L65">
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5AEF7E3B-027E-48F1-9620-D4413DF40490}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L57:L67">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7B910169-92BE-420A-A2EC-668F2F70CBF6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D73:D83">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{34EED8B1-E658-46DF-A583-5C1152103F2C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D310E4DC-B88B-4EEC-B3F1-29BBE07012D0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72:L72 D72:E72 K75:L75 E73:E83 K74 K82:L83 K76:K81">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{35877C9A-6B39-4A6D-BC13-C128CDDDB130}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73:F83">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EC726271-19DC-4051-A4D3-84ECF3C69BA8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G72:G83">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{55053CFB-7BA4-4819-A5BA-8DB439BD406B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72:H83">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6622B835-86A9-4D2E-BFF0-EAADB4006AC4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73:I83">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9316F3A0-B146-4757-94CF-D4E3CC8DB9FC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J72:J83">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8EEAC486-55C9-4AE2-9C33-662313B69441}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L73:L74">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E5587B46-107A-4D7F-8959-F3D2B5D5B9ED}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76:L81">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{97B0D3C3-5278-449E-9BCB-B4A5F69FB462}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L73:L83">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3E87C20E-1121-46A5-A38C-C5ED2B94F69F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57:D67">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FD8CADF4-6A6B-46BC-A242-1826A5BBEA5B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D33">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0829646D-B0EA-4943-9374-3FF6742F96DF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E98D1A6E-F6B1-4BA9-B779-9819B6034BE5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:N17">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{209F7202-9E39-4CA7-B78C-56105F1E476F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7:K17">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2E230540-D05F-4565-950E-DB843F2920F8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -3928,7 +4815,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I39:I51 J40:K50 I20 K39 I53:I54 I70:I1048576</xm:sqref>
+          <xm:sqref>I39:I51 J40:K50 I20 K39 I53:I54 I70 I86:I1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BB2EB6A5-6AB7-418B-B4EC-2CEA3A48BD81}">
@@ -4011,7 +4898,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H38:H51 H20 H53:H54 H70:H1048576</xm:sqref>
+          <xm:sqref>H38:H51 H20 H53:H54 H70 H86:H1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{248A10D3-B8FE-465B-83E1-C1E4AC2CCDF3}">
@@ -4088,17 +4975,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>J6:J17</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{476397F3-E88D-4891-9A86-1454E9281DAC}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D23:D33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{70B5C366-A4BF-4187-8AA5-731F000DF777}">
@@ -4188,17 +5064,6 @@
           <xm:sqref>J22:J33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{42F8FBF0-D54C-4CD6-9F3F-B8267C763866}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D57:D67</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D20CE542-556C-44F0-9053-0B35F8C4A47D}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
@@ -4207,7 +5072,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K57:L57</xm:sqref>
+          <xm:sqref>K57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3079829D-DE73-4826-9A91-D728D0F77E55}">
@@ -4218,7 +5083,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K56:L56 D56:E56 K58:L67 E57:E67</xm:sqref>
+          <xm:sqref>K56:L56 D56:E56 K59:L59 E57:E67 K58 K66:L67 K60:K65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F5B1D25D-9B0D-4D07-AA83-2EAFF307BDDD}">
@@ -4285,6 +5150,231 @@
           </x14:cfRule>
           <xm:sqref>J56:J67</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CCF4670A-9CCA-4C1C-967F-45C4C21C6884}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L57:L58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5AEF7E3B-027E-48F1-9620-D4413DF40490}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L60:L65</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7B910169-92BE-420A-A2EC-668F2F70CBF6}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L57:L67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{34EED8B1-E658-46DF-A583-5C1152103F2C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D73:D83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D310E4DC-B88B-4EEC-B3F1-29BBE07012D0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K73</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{35877C9A-6B39-4A6D-BC13-C128CDDDB130}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K72:L72 D72:E72 K75:L75 E73:E83 K74 K82:L83 K76:K81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EC726271-19DC-4051-A4D3-84ECF3C69BA8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F73:F83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{55053CFB-7BA4-4819-A5BA-8DB439BD406B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G72:G83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6622B835-86A9-4D2E-BFF0-EAADB4006AC4}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H72:H83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9316F3A0-B146-4757-94CF-D4E3CC8DB9FC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I73:I83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8EEAC486-55C9-4AE2-9C33-662313B69441}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J72:J83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E5587B46-107A-4D7F-8959-F3D2B5D5B9ED}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L73:L74</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{97B0D3C3-5278-449E-9BCB-B4A5F69FB462}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L76:L81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3E87C20E-1121-46A5-A38C-C5ED2B94F69F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L73:L83</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FD8CADF4-6A6B-46BC-A242-1826A5BBEA5B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D57:D67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0829646D-B0EA-4943-9374-3FF6742F96DF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D23:D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E98D1A6E-F6B1-4BA9-B779-9819B6034BE5}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{209F7202-9E39-4CA7-B78C-56105F1E476F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N8:N17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2E230540-D05F-4565-950E-DB843F2920F8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K7:K17</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -4308,7 +5398,7 @@
   <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4419,12 +5509,137 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Pintax config v4 try1
</commit_message>
<xml_diff>
--- a/Backtesting_PTStratx_search_settings.xlsx
+++ b/Backtesting_PTStratx_search_settings.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RESULT" sheetId="2" r:id="rId1"/>
     <sheet name="CryptoZen 1.0" sheetId="5" r:id="rId2"/>
     <sheet name="El Toro 1.0" sheetId="3" r:id="rId3"/>
     <sheet name="El Dorado 1.0" sheetId="4" r:id="rId4"/>
-    <sheet name="Test Trigger drop" sheetId="1" r:id="rId5"/>
+    <sheet name="El Dorado 2.0" sheetId="6" r:id="rId5"/>
+    <sheet name="Test Trigger drop" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -153,12 +154,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C88" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>toytoy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification du captial pour TradingView qui à du mal avec beaucoup d'unité pour par exemple ICX / ONT etc</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="242">
   <si>
     <t>Search Price  Trigger</t>
   </si>
@@ -712,6 +737,475 @@
   </si>
   <si>
     <t>El Dorado 1.0</t>
+  </si>
+  <si>
+    <t>El Dorado 2.0</t>
+  </si>
+  <si>
+    <t>DEFAULT_DCA_buy_trigger = -3</t>
+  </si>
+  <si>
+    <r>
+      <t>DEFAULT_buy_min_change_percentage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DEFAULT_buy_max_change_percentage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "------ PTStratX 1.0.8 - Easy Strats and more ---------": "1.0.8",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "------ for Profittrailer 2 and other Bots  -------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "------------------------- BUY -------------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_A_buy_strategy": "SMACROSS",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_A_buy_value": "0.01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_A_buy_value_limit": "20",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "-------------------------------------------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_B_buy_strategy": "EMAGAIN",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_B_buy_value": "0.01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_B_buy_value_limit": "20",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "--------------------------------------------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_C_buy_strategy": "RSI",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_C_buy_value": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_C_buy_value_limit": "30",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_D_buy_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_D_buy_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_D_buy_value_limit": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_E_buy_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_E_buy_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_E_buy_value_limit": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "------------- INDICATOR PARAMETERS -------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "EMA_slow_length (blue)": "13",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "EMA_fast_length (green)": "8",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "EMA_cross_candles": "12",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "EMA_candle_period (in Sec)": "  300s / 5m",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SMA_slow_length (blue)": "55",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SMA_fast_length (green)": "21",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SMA_cross_candles": "4",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SMA_candle_period (in Sec)": " 3600s / 1h",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "BB_length": "20",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "BB_std": "2",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "BB_candle_period (in Sec)": "  900s / 15m",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "RSI_length": "2",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "RSI_candle_period (in Sec)": "  300s / 5m",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "STOCH_length": "14",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "STOCH_candle_period (in Sec)": "  300s / 5m",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "MACD_fast_length": "12",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "MACD_slow_length": "26",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "MACD_signal": "9",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "MACD_candle_period (in Sec)": "14400s / 4h",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "LOWBB Price Trigger": "low",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "HIGHBB Price Trigger": "high",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "GAIN Price Trigger": "high",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "EMAGAIN Price Trigger": "close",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SMAGAIN Price Trigger": "close",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "----------SOM Parameters-------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_rebuy_timeout (in min)": "5",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_rebuy_timeout (in min)": "10",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "min/max_change_percentage_length (PT use only 1440m / 1d) (in min)": "1440",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_buy_min_change_percentage": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_buy_max_change_percentage": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_min_change_percentage": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_max_change_percentage": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "price_drop_trigger (in %)": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "price_drop_recover_trigger (in %)": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "price_rise_trigger (in %)": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "price_rise_recover_trigger (in %)": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "price_trigger_market": "BTC",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SOM_trigger_length (5 Minute Candles * X)": "12",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "----------------------- DCA BUY ----------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_A_buy_strategy": "SMACROSS",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_A_buy_value": "0.01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_A_buy_value_limit": "20",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_B_buy_strategy": "EMAGAIN",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_B_buy_value": "0.01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_B_buy_value_limit": "20",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_C_buy_strategy": "RSI",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_C_buy_value": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_C_buy_value_limit": "30",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_D_buy_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_D_buy_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_D_buy_value_limit": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_E_buy_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_E_buy_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_E_buy_value_limit": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "------------------ ANDERSON DCA -------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_enabled": true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_max_buy_times": "5",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "SOM_DCA_buy_trigger": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_ignore_sell_only_mode": true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger": "-3",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_1": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_2": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_3": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_4": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_5": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_6": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_7": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_8": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_trigger_9": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_1": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_2": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_3": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_4": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_5": "100",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_6": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_7": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_8": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_buy_percentage_9": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "------------------------- SELL -------------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_A_sell_strategy (GAIN is mandatory)": "GAIN",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_A_sell_value": "2",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_B_sell_strategy": "RSI",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_B_sell_value": "80",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_C_sell_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_C_sell_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_D_sell_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_D_sell_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_E_sell_strategy": "--",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_E_sell_value": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_stop_loss_trigger": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "--------------------- TRAILING ----------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_trailing_buy": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_DCA_trailing_buy": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DEFAULT_trailing_profit": "0.25",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "-------------------- BACKTEST ----------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "From Minute": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "From Hour": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "From Month": "9",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "From Day": "1",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "From Year": "2017",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "To Month": "1",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "To Day": "1",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "To Year": "9999",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "--------------------- PLOTTING ----------------------": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Setting Debug Mode with letters; DCA=orange, Buy=green": true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat ALL = true with Bars (green)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat ALL = true with Arrows (green)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat A = true with Letters (green Letter A)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat B = true with Letters (green Letter B)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat C = true with Letters (green Letter C)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat D = true with Letters (green Letter D)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Buystrat E = true with Letters (green Letter E)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show DCA Buystrat ALL = true with Bars (orange)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show DCA Buystrat A = true with Letters (orange Letter A)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show DCA Buystrat B = true with Letters (orange Letter B)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show DCA Buystrat C = true with Letters (orange Letter C)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show DCA Buystrat D = true with Letters (orange Letter D)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show DCA Buystrat E = true with Letters (orange Letter E)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show SellStrat All = true with Bars (red)": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Show Trailing Debug Informations": false</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>ETHBTC up  55 à 67%</t>
   </si>
 </sst>
 </file>
@@ -896,7 +1390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,12 +1459,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1016,13 +1504,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="83">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1030,35 +1577,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1095,6 +1623,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1110,24 +1642,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1157,6 +1671,20 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
@@ -1204,6 +1732,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1214,6 +1756,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1243,6 +1789,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1309,127 +1859,148 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A39:K50" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A39:K50" totalsRowShown="0" dataDxfId="82">
   <autoFilter ref="A39:K50"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Name Settings" dataDxfId="68"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="67"/>
-    <tableColumn id="11" name="Captial" dataDxfId="66"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="65"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="64"/>
-    <tableColumn id="2" name="DCA blocked (J)" dataDxfId="63"/>
-    <tableColumn id="5" name="Blocked today " dataDxfId="62"/>
-    <tableColumn id="8" name="Net Profit " dataDxfId="61"/>
-    <tableColumn id="9" name="Closed Trades2" dataDxfId="60"/>
-    <tableColumn id="4" name="DCA blocked (J)2" dataDxfId="59"/>
-    <tableColumn id="10" name="Blocked today" dataDxfId="58"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="81"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="80"/>
+    <tableColumn id="11" name="Captial" dataDxfId="79"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="78"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="77"/>
+    <tableColumn id="2" name="DCA blocked (J)" dataDxfId="76"/>
+    <tableColumn id="5" name="Blocked today " dataDxfId="75"/>
+    <tableColumn id="8" name="Net Profit " dataDxfId="74"/>
+    <tableColumn id="9" name="Closed Trades2" dataDxfId="73"/>
+    <tableColumn id="4" name="DCA blocked (J)2" dataDxfId="72"/>
+    <tableColumn id="10" name="Blocked today" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau25" displayName="Tableau25" ref="A6:L17" totalsRowShown="0" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau25" displayName="Tableau25" ref="A6:L17" totalsRowShown="0" dataDxfId="70">
   <autoFilter ref="A6:L17"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="56"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="55"/>
-    <tableColumn id="11" name="Captial" dataDxfId="54"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="1"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="53"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="52"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="51"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="50"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="49"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="48"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="47"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="0"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="69"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="68"/>
+    <tableColumn id="11" name="Captial" dataDxfId="67"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="66"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="65"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="64"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="63"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="62"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="61"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="60"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="59"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau257" displayName="Tableau257" ref="A22:L33" totalsRowShown="0" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau257" displayName="Tableau257" ref="A22:L33" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A22:L33"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="45"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="44"/>
-    <tableColumn id="11" name="Captial" dataDxfId="43"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="2"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="42"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="41"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="40"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="39"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="38"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="37"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="36"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="35"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="56"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="55"/>
+    <tableColumn id="11" name="Captial" dataDxfId="54"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="53"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="52"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="51"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="50"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="49"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="48"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="47"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="46"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau256" displayName="Tableau256" ref="A56:L67" totalsRowShown="0" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau256" displayName="Tableau256" ref="A56:L67" totalsRowShown="0" dataDxfId="44">
   <autoFilter ref="A56:L67"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="33"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="32"/>
-    <tableColumn id="11" name="Captial" dataDxfId="31"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="3"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="30"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="29"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="28"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="27"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="26"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="25"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="24"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="17"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="43"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="42"/>
+    <tableColumn id="11" name="Captial" dataDxfId="41"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="40"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="39"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="38"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="37"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="36"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="35"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="34"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="33"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau2568" displayName="Tableau2568" ref="A72:L83" totalsRowShown="0" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau2568" displayName="Tableau2568" ref="A72:L83" totalsRowShown="0" dataDxfId="31">
   <autoFilter ref="A72:L83"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Name Settings" dataDxfId="15"/>
-    <tableColumn id="3" name="Crypto" dataDxfId="14"/>
-    <tableColumn id="11" name="Captial" dataDxfId="13"/>
-    <tableColumn id="6" name="Net Profit (%)" dataDxfId="4"/>
-    <tableColumn id="7" name="Closed Trades" dataDxfId="12"/>
-    <tableColumn id="2" name="% Profitable" dataDxfId="11"/>
-    <tableColumn id="5" name="Profit Factor" dataDxfId="10"/>
-    <tableColumn id="8" name="Max DrawDown" dataDxfId="9"/>
-    <tableColumn id="9" name="Avg Trade" dataDxfId="8"/>
-    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="7"/>
-    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="6"/>
-    <tableColumn id="12" name="Blocked today " dataDxfId="5"/>
+    <tableColumn id="1" name="Name Settings" dataDxfId="30"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="29"/>
+    <tableColumn id="11" name="Captial" dataDxfId="28"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="27"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="26"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="25"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="24"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="23"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="22"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="21"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="20"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C39" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A2:C39"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="lenght" dataDxfId="21"/>
-    <tableColumn id="2" name="price_drop_trigger" dataDxfId="20"/>
-    <tableColumn id="3" name="ETHBTC - 2h" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau25689" displayName="Tableau25689" ref="A88:L99" totalsRowShown="0" dataDxfId="18">
+  <autoFilter ref="A88:L99"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Name Settings" dataDxfId="17"/>
+    <tableColumn id="3" name="Crypto" dataDxfId="16"/>
+    <tableColumn id="11" name="Captial" dataDxfId="15"/>
+    <tableColumn id="6" name="Net Profit (%)" dataDxfId="14"/>
+    <tableColumn id="7" name="Closed Trades" dataDxfId="13"/>
+    <tableColumn id="2" name="% Profitable" dataDxfId="12"/>
+    <tableColumn id="5" name="Profit Factor" dataDxfId="11"/>
+    <tableColumn id="8" name="Max DrawDown" dataDxfId="10"/>
+    <tableColumn id="9" name="Avg Trade" dataDxfId="9"/>
+    <tableColumn id="4" name="Avg Bars in Trade" dataDxfId="8"/>
+    <tableColumn id="10" name="DCA blocked (J)" dataDxfId="7"/>
+    <tableColumn id="12" name="Blocked today " dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:C39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:C39"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="lenght" dataDxfId="3"/>
+    <tableColumn id="2" name="price_drop_trigger" dataDxfId="2"/>
+    <tableColumn id="3" name="ETHBTC - 2h" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="H5:I14" totalsRowShown="0">
   <autoFilter ref="H5:I14"/>
   <tableColumns count="2">
     <tableColumn id="1" name="base 5min"/>
-    <tableColumn id="2" name="candles" dataDxfId="18">
+    <tableColumn id="2" name="candles" dataDxfId="0">
       <calculatedColumnFormula>G6*60/Tableau3[[#This Row],[base 5min]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1700,10 +2271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1751,20 +2322,20 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -1804,7 +2375,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -1814,7 +2385,7 @@
       <c r="C7" s="15">
         <v>2000000</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="28">
         <v>0.66</v>
       </c>
       <c r="E7" s="17">
@@ -1838,12 +2409,12 @@
       <c r="K7" s="21">
         <v>22</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="28">
         <v>-5</v>
       </c>
-      <c r="N7" s="36"/>
-    </row>
-    <row r="8" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>52</v>
       </c>
@@ -1853,7 +2424,7 @@
       <c r="C8" s="15">
         <v>2000000</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="28">
         <v>0.08</v>
       </c>
       <c r="E8" s="17">
@@ -1877,12 +2448,12 @@
       <c r="K8" s="21">
         <v>10</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="28">
         <v>-5</v>
       </c>
-      <c r="N8" s="36"/>
-    </row>
-    <row r="9" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N8" s="34"/>
+    </row>
+    <row r="9" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>52</v>
       </c>
@@ -1892,7 +2463,7 @@
       <c r="C9" s="15">
         <v>200000</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="28">
         <v>0.21</v>
       </c>
       <c r="E9" s="17">
@@ -1916,12 +2487,12 @@
       <c r="K9" s="21">
         <v>31</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="28">
         <v>0</v>
       </c>
-      <c r="N9" s="35"/>
-    </row>
-    <row r="10" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N9" s="33"/>
+    </row>
+    <row r="10" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +2502,7 @@
       <c r="C10" s="15">
         <v>200000</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>1.06</v>
       </c>
       <c r="E10" s="17">
@@ -1955,12 +2526,12 @@
       <c r="K10" s="21">
         <v>5</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="28">
         <v>0</v>
       </c>
-      <c r="N10" s="35"/>
-    </row>
-    <row r="11" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N10" s="33"/>
+    </row>
+    <row r="11" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>52</v>
       </c>
@@ -1970,7 +2541,7 @@
       <c r="C11" s="15">
         <v>200000</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="28">
         <v>0.49</v>
       </c>
       <c r="E11" s="17">
@@ -1994,12 +2565,12 @@
       <c r="K11" s="21">
         <v>3</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="28">
         <v>0</v>
       </c>
-      <c r="N11" s="35"/>
-    </row>
-    <row r="12" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N11" s="33"/>
+    </row>
+    <row r="12" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>52</v>
       </c>
@@ -2009,7 +2580,7 @@
       <c r="C12" s="15">
         <v>200000</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="28">
         <v>0.72</v>
       </c>
       <c r="E12" s="17">
@@ -2033,12 +2604,12 @@
       <c r="K12" s="21">
         <v>45</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="28">
         <v>-30</v>
       </c>
-      <c r="N12" s="36"/>
-    </row>
-    <row r="13" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N12" s="34"/>
+    </row>
+    <row r="13" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>52</v>
       </c>
@@ -2048,7 +2619,7 @@
       <c r="C13" s="15">
         <v>200000</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>0.13</v>
       </c>
       <c r="E13" s="17">
@@ -2072,12 +2643,12 @@
       <c r="K13" s="21">
         <v>4</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="28">
         <v>0</v>
       </c>
-      <c r="N13" s="35"/>
-    </row>
-    <row r="14" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N13" s="33"/>
+    </row>
+    <row r="14" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>52</v>
       </c>
@@ -2087,7 +2658,7 @@
       <c r="C14" s="15">
         <v>200000</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>5.18</v>
       </c>
       <c r="E14" s="17">
@@ -2111,12 +2682,12 @@
       <c r="K14" s="21">
         <v>3</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="28">
         <v>0</v>
       </c>
-      <c r="N14" s="35"/>
-    </row>
-    <row r="15" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N14" s="33"/>
+    </row>
+    <row r="15" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>52</v>
       </c>
@@ -2126,7 +2697,7 @@
       <c r="C15" s="15">
         <v>200000</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="28">
         <v>1.78</v>
       </c>
       <c r="E15" s="17">
@@ -2150,12 +2721,12 @@
       <c r="K15" s="21">
         <v>4</v>
       </c>
-      <c r="L15" s="30">
+      <c r="L15" s="28">
         <v>0</v>
       </c>
-      <c r="N15" s="35"/>
-    </row>
-    <row r="16" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N15" s="33"/>
+    </row>
+    <row r="16" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>52</v>
       </c>
@@ -2165,7 +2736,7 @@
       <c r="C16" s="15">
         <v>20000</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <v>0.68</v>
       </c>
       <c r="E16" s="17">
@@ -2189,12 +2760,12 @@
       <c r="K16" s="21">
         <v>15</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="28">
         <v>0</v>
       </c>
-      <c r="N16" s="36"/>
-    </row>
-    <row r="17" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="N16" s="34"/>
+    </row>
+    <row r="17" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>52</v>
       </c>
@@ -2204,7 +2775,7 @@
       <c r="C17" s="15">
         <v>20000</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="28">
         <v>0.4</v>
       </c>
       <c r="E17" s="17">
@@ -2228,12 +2799,12 @@
       <c r="K17" s="22">
         <v>22</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="29">
         <v>-20</v>
       </c>
-      <c r="N17" s="36"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="34"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="15"/>
@@ -2245,61 +2816,61 @@
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="36">
         <f>AVERAGE(Tableau25[Net Profit (%)])</f>
         <v>1.0354545454545454</v>
       </c>
-      <c r="E19" s="39">
+      <c r="E19" s="37">
         <f>AVERAGE(Tableau25[Closed Trades])</f>
         <v>45.272727272727273</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="37">
         <f>AVERAGE(Tableau25[% Profitable])</f>
         <v>50.899090909090908</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="37">
         <f>AVERAGE(Tableau25[Profit Factor])</f>
         <v>1.922181818181818</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="37">
         <f>AVERAGE(Tableau25[Max DrawDown])</f>
         <v>1.1969999999999998</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="37">
         <f>AVERAGE(Tableau25[Avg Trade])</f>
         <v>2.2727272727272724E-2</v>
       </c>
-      <c r="J19" s="39">
+      <c r="J19" s="37">
         <f>AVERAGE(Tableau25[Avg Bars in Trade])</f>
         <v>13.182727272727272</v>
       </c>
-      <c r="K19" s="39">
+      <c r="K19" s="37">
         <f>AVERAGE(Tableau25[DCA blocked (J)])</f>
         <v>14.909090909090908</v>
       </c>
-      <c r="L19" s="40">
+      <c r="L19" s="38">
         <f>AVERAGE(Tableau25[[Blocked today ]])</f>
         <v>-5.4545454545454541</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
@@ -2571,18 +3142,18 @@
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="40"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="38"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H36" s="13"/>
@@ -2597,18 +3168,18 @@
       <c r="K37" s="16"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28" t="s">
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -2986,32 +3557,32 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
-      <c r="C52" s="41" t="s">
+      <c r="C52" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="40">
         <f>AVERAGE(Tableau2[Net Profit (%)])</f>
         <v>2.4087499999999998E-2</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="41">
         <f>AVERAGE(Tableau2[Closed Trades])</f>
         <v>62.125</v>
       </c>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43">
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41">
         <f>AVERAGE(Tableau2[[Net Profit ]])</f>
         <v>4.4745454545454555</v>
       </c>
-      <c r="I52" s="43">
+      <c r="I52" s="41">
         <f>AVERAGE(Tableau2[Closed Trades2])</f>
         <v>120.72727272727273</v>
       </c>
-      <c r="J52" s="43">
+      <c r="J52" s="41">
         <f>AVERAGE(Tableau2[DCA blocked (J)2])</f>
         <v>67.818181818181813</v>
       </c>
-      <c r="K52" s="44">
+      <c r="K52" s="42">
         <f>AVERAGE(Tableau2[Blocked today])</f>
         <v>-0.17181818181818184</v>
       </c>
@@ -3026,20 +3597,20 @@
       <c r="I53" s="2"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="28"/>
-      <c r="K55" s="28"/>
-      <c r="L55" s="28"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="45"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
@@ -3089,7 +3660,7 @@
       <c r="C57" s="15">
         <v>2000000</v>
       </c>
-      <c r="D57" s="30">
+      <c r="D57" s="28">
         <v>2.88</v>
       </c>
       <c r="E57" s="20">
@@ -3113,7 +3684,7 @@
       <c r="K57" s="21">
         <v>120</v>
       </c>
-      <c r="L57" s="30">
+      <c r="L57" s="28">
         <v>-32</v>
       </c>
     </row>
@@ -3127,7 +3698,7 @@
       <c r="C58" s="15">
         <v>2000000</v>
       </c>
-      <c r="D58" s="30">
+      <c r="D58" s="28">
         <v>2.89</v>
       </c>
       <c r="E58" s="20">
@@ -3151,7 +3722,7 @@
       <c r="K58" s="21">
         <v>54</v>
       </c>
-      <c r="L58" s="30">
+      <c r="L58" s="28">
         <v>-8</v>
       </c>
     </row>
@@ -3165,7 +3736,7 @@
       <c r="C59" s="15">
         <v>200000</v>
       </c>
-      <c r="D59" s="30">
+      <c r="D59" s="28">
         <v>5.33</v>
       </c>
       <c r="E59" s="20">
@@ -3189,7 +3760,7 @@
       <c r="K59" s="21">
         <v>75</v>
       </c>
-      <c r="L59" s="30">
+      <c r="L59" s="28">
         <v>-7</v>
       </c>
     </row>
@@ -3203,7 +3774,7 @@
       <c r="C60" s="15">
         <v>200000</v>
       </c>
-      <c r="D60" s="30">
+      <c r="D60" s="28">
         <v>2.62</v>
       </c>
       <c r="E60" s="20">
@@ -3227,7 +3798,7 @@
       <c r="K60" s="21">
         <v>125</v>
       </c>
-      <c r="L60" s="30">
+      <c r="L60" s="28">
         <v>-30</v>
       </c>
     </row>
@@ -3241,7 +3812,7 @@
       <c r="C61" s="15">
         <v>200000</v>
       </c>
-      <c r="D61" s="30">
+      <c r="D61" s="28">
         <v>2.48</v>
       </c>
       <c r="E61" s="20">
@@ -3265,7 +3836,7 @@
       <c r="K61" s="21">
         <v>24</v>
       </c>
-      <c r="L61" s="30">
+      <c r="L61" s="28">
         <v>-22</v>
       </c>
     </row>
@@ -3279,7 +3850,7 @@
       <c r="C62" s="15">
         <v>200000</v>
       </c>
-      <c r="D62" s="30">
+      <c r="D62" s="28">
         <v>2.5</v>
       </c>
       <c r="E62" s="20">
@@ -3303,7 +3874,7 @@
       <c r="K62" s="21">
         <v>66</v>
       </c>
-      <c r="L62" s="30">
+      <c r="L62" s="28">
         <v>-37</v>
       </c>
     </row>
@@ -3317,7 +3888,7 @@
       <c r="C63" s="15">
         <v>200000</v>
       </c>
-      <c r="D63" s="30">
+      <c r="D63" s="28">
         <v>3.41</v>
       </c>
       <c r="E63" s="20">
@@ -3341,7 +3912,7 @@
       <c r="K63" s="21">
         <v>32</v>
       </c>
-      <c r="L63" s="30">
+      <c r="L63" s="28">
         <v>-5</v>
       </c>
     </row>
@@ -3355,7 +3926,7 @@
       <c r="C64" s="15">
         <v>200000</v>
       </c>
-      <c r="D64" s="30">
+      <c r="D64" s="28">
         <v>2.36</v>
       </c>
       <c r="E64" s="20">
@@ -3379,7 +3950,7 @@
       <c r="K64" s="21">
         <v>129</v>
       </c>
-      <c r="L64" s="30">
+      <c r="L64" s="28">
         <v>-4</v>
       </c>
     </row>
@@ -3393,7 +3964,7 @@
       <c r="C65" s="15">
         <v>200000</v>
       </c>
-      <c r="D65" s="30">
+      <c r="D65" s="28">
         <v>1.59</v>
       </c>
       <c r="E65" s="20">
@@ -3417,7 +3988,7 @@
       <c r="K65" s="21">
         <v>177</v>
       </c>
-      <c r="L65" s="30">
+      <c r="L65" s="28">
         <v>-50</v>
       </c>
     </row>
@@ -3431,7 +4002,7 @@
       <c r="C66" s="15">
         <v>20000</v>
       </c>
-      <c r="D66" s="30">
+      <c r="D66" s="28">
         <v>4.01</v>
       </c>
       <c r="E66" s="20">
@@ -3455,7 +4026,7 @@
       <c r="K66" s="21">
         <v>73</v>
       </c>
-      <c r="L66" s="30">
+      <c r="L66" s="28">
         <v>-16</v>
       </c>
     </row>
@@ -3469,7 +4040,7 @@
       <c r="C67" s="15">
         <v>20000</v>
       </c>
-      <c r="D67" s="30">
+      <c r="D67" s="28">
         <v>1.77</v>
       </c>
       <c r="E67" s="20">
@@ -3493,7 +4064,7 @@
       <c r="K67" s="22">
         <v>25</v>
       </c>
-      <c r="L67" s="31">
+      <c r="L67" s="29">
         <v>-10</v>
       </c>
     </row>
@@ -3509,61 +4080,61 @@
     <row r="69" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="20"/>
-      <c r="C69" s="37" t="s">
+      <c r="C69" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D69" s="38">
+      <c r="D69" s="36">
         <f>AVERAGE(Tableau256[Net Profit (%)])</f>
         <v>2.8945454545454545</v>
       </c>
-      <c r="E69" s="39">
+      <c r="E69" s="37">
         <f>AVERAGE(Tableau256[Closed Trades])</f>
         <v>48.454545454545453</v>
       </c>
-      <c r="F69" s="39">
+      <c r="F69" s="37">
         <f>AVERAGE(Tableau256[% Profitable])</f>
         <v>79.979090909090914</v>
       </c>
-      <c r="G69" s="39">
+      <c r="G69" s="37">
         <f>AVERAGE(Tableau256[Profit Factor])</f>
         <v>5.058727272727273</v>
       </c>
-      <c r="H69" s="39">
+      <c r="H69" s="37">
         <f>AVERAGE(Tableau256[Max DrawDown])</f>
         <v>0.56363636363636371</v>
       </c>
-      <c r="I69" s="39">
+      <c r="I69" s="37">
         <f>AVERAGE(Tableau256[Avg Trade])</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J69" s="39">
+      <c r="J69" s="37">
         <f>AVERAGE(Tableau256[Avg Bars in Trade])</f>
         <v>88.63636363636364</v>
       </c>
-      <c r="K69" s="39">
+      <c r="K69" s="37">
         <f>AVERAGE(Tableau256[DCA blocked (J)])</f>
         <v>81.818181818181813</v>
       </c>
-      <c r="L69" s="40">
+      <c r="L69" s="38">
         <f>AVERAGE(Tableau256[[Blocked today ]])</f>
         <v>-20.09090909090909</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
+      <c r="A71" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="28"/>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
+      <c r="B71" s="45"/>
+      <c r="C71" s="45"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="45"/>
+      <c r="G71" s="45"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="45"/>
+      <c r="J71" s="45"/>
+      <c r="K71" s="45"/>
+      <c r="L71" s="45"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
@@ -3613,7 +4184,7 @@
       <c r="C73" s="15">
         <v>2000000</v>
       </c>
-      <c r="D73" s="30">
+      <c r="D73" s="28">
         <v>16.48</v>
       </c>
       <c r="E73" s="27">
@@ -3637,7 +4208,7 @@
       <c r="K73" s="21">
         <v>53</v>
       </c>
-      <c r="L73" s="30">
+      <c r="L73" s="28">
         <v>-6</v>
       </c>
     </row>
@@ -3651,7 +4222,7 @@
       <c r="C74" s="15">
         <v>2000000</v>
       </c>
-      <c r="D74" s="30">
+      <c r="D74" s="28">
         <v>55.57</v>
       </c>
       <c r="E74" s="27">
@@ -3675,7 +4246,7 @@
       <c r="K74" s="21">
         <v>30</v>
       </c>
-      <c r="L74" s="30">
+      <c r="L74" s="28">
         <v>-2</v>
       </c>
     </row>
@@ -3689,7 +4260,7 @@
       <c r="C75" s="15">
         <v>200000</v>
       </c>
-      <c r="D75" s="30">
+      <c r="D75" s="28">
         <v>20.079999999999998</v>
       </c>
       <c r="E75" s="27">
@@ -3713,7 +4284,7 @@
       <c r="K75" s="21">
         <v>23</v>
       </c>
-      <c r="L75" s="30">
+      <c r="L75" s="28">
         <v>0</v>
       </c>
     </row>
@@ -3727,7 +4298,7 @@
       <c r="C76" s="15">
         <v>200000</v>
       </c>
-      <c r="D76" s="30">
+      <c r="D76" s="28">
         <v>10.66</v>
       </c>
       <c r="E76" s="27">
@@ -3751,7 +4322,7 @@
       <c r="K76" s="21">
         <v>47</v>
       </c>
-      <c r="L76" s="30">
+      <c r="L76" s="28">
         <v>-8</v>
       </c>
     </row>
@@ -3765,7 +4336,7 @@
       <c r="C77" s="15">
         <v>200000</v>
       </c>
-      <c r="D77" s="30">
+      <c r="D77" s="28">
         <v>3.81</v>
       </c>
       <c r="E77" s="27">
@@ -3789,7 +4360,7 @@
       <c r="K77" s="21">
         <v>25</v>
       </c>
-      <c r="L77" s="30">
+      <c r="L77" s="28">
         <v>-18</v>
       </c>
     </row>
@@ -3803,7 +4374,7 @@
       <c r="C78" s="15">
         <v>200000</v>
       </c>
-      <c r="D78" s="30">
+      <c r="D78" s="28">
         <v>7.25</v>
       </c>
       <c r="E78" s="27">
@@ -3827,7 +4398,7 @@
       <c r="K78" s="21">
         <v>16</v>
       </c>
-      <c r="L78" s="30">
+      <c r="L78" s="28">
         <v>0</v>
       </c>
     </row>
@@ -3841,7 +4412,7 @@
       <c r="C79" s="15">
         <v>200000</v>
       </c>
-      <c r="D79" s="30">
+      <c r="D79" s="28">
         <v>17.149999999999999</v>
       </c>
       <c r="E79" s="27">
@@ -3865,7 +4436,7 @@
       <c r="K79" s="21">
         <v>29</v>
       </c>
-      <c r="L79" s="30">
+      <c r="L79" s="28">
         <v>0</v>
       </c>
     </row>
@@ -3879,7 +4450,7 @@
       <c r="C80" s="15">
         <v>200000</v>
       </c>
-      <c r="D80" s="30">
+      <c r="D80" s="28">
         <v>11.11</v>
       </c>
       <c r="E80" s="27">
@@ -3903,11 +4474,11 @@
       <c r="K80" s="21">
         <v>51</v>
       </c>
-      <c r="L80" s="30">
+      <c r="L80" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
         <v>74</v>
       </c>
@@ -3917,7 +4488,7 @@
       <c r="C81" s="15">
         <v>200000</v>
       </c>
-      <c r="D81" s="30">
+      <c r="D81" s="28">
         <v>10.66</v>
       </c>
       <c r="E81" s="27">
@@ -3941,11 +4512,11 @@
       <c r="K81" s="21">
         <v>25</v>
       </c>
-      <c r="L81" s="30">
+      <c r="L81" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
         <v>74</v>
       </c>
@@ -3955,7 +4526,7 @@
       <c r="C82" s="15">
         <v>20000</v>
       </c>
-      <c r="D82" s="30">
+      <c r="D82" s="28">
         <v>5.57</v>
       </c>
       <c r="E82" s="27">
@@ -3979,11 +4550,11 @@
       <c r="K82" s="21">
         <v>26</v>
       </c>
-      <c r="L82" s="30">
+      <c r="L82" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
         <v>74</v>
       </c>
@@ -3993,7 +4564,7 @@
       <c r="C83" s="15">
         <v>20000</v>
       </c>
-      <c r="D83" s="30">
+      <c r="D83" s="28">
         <v>4.59</v>
       </c>
       <c r="E83" s="27">
@@ -4017,11 +4588,11 @@
       <c r="K83" s="22">
         <v>25</v>
       </c>
-      <c r="L83" s="31">
+      <c r="L83" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="27"/>
       <c r="B84" s="27"/>
       <c r="C84" s="15"/>
@@ -4030,52 +4601,397 @@
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="27"/>
       <c r="B85" s="27"/>
-      <c r="C85" s="37" t="s">
+      <c r="C85" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D85" s="38">
+      <c r="D85" s="36">
         <f>AVERAGE(Tableau2568[Net Profit (%)])</f>
         <v>14.811818181818182</v>
       </c>
-      <c r="E85" s="39">
+      <c r="E85" s="37">
         <f>AVERAGE(Tableau2568[Closed Trades])</f>
         <v>96.090909090909093</v>
       </c>
-      <c r="F85" s="39">
+      <c r="F85" s="37">
         <f>AVERAGE(Tableau2568[% Profitable])</f>
         <v>1486.3245454545452</v>
       </c>
-      <c r="G85" s="39">
+      <c r="G85" s="37">
         <f>AVERAGE(Tableau2568[Profit Factor])</f>
         <v>3.1806363636363639</v>
       </c>
-      <c r="H85" s="39">
+      <c r="H85" s="37">
         <f>AVERAGE(Tableau2568[Max DrawDown])</f>
         <v>3.6843636363636363</v>
       </c>
-      <c r="I85" s="39">
+      <c r="I85" s="37">
         <f>AVERAGE(Tableau2568[Avg Trade])</f>
         <v>0.14363636363636367</v>
       </c>
-      <c r="J85" s="39">
+      <c r="J85" s="37">
         <f>AVERAGE(Tableau2568[Avg Bars in Trade])</f>
         <v>44.272727272727273</v>
       </c>
-      <c r="K85" s="39">
+      <c r="K85" s="37">
         <f>AVERAGE(Tableau2568[DCA blocked (J)])</f>
         <v>31.818181818181817</v>
       </c>
-      <c r="L85" s="40">
+      <c r="L85" s="38">
         <f>AVERAGE(Tableau2568[[Blocked today ]])</f>
         <v>-3.0909090909090908</v>
       </c>
     </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B87" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C87" s="45"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="45"/>
+      <c r="J87" s="45"/>
+      <c r="K87" s="45"/>
+      <c r="L87" s="45"/>
+      <c r="M87" s="45"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E88" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F88" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G88" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="H88" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="I88" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="J88" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="K88" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="L88" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B89" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="15">
+        <v>2000000</v>
+      </c>
+      <c r="D89" s="28"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="44"/>
+      <c r="I89" s="44"/>
+      <c r="J89" s="44"/>
+      <c r="K89" s="21"/>
+      <c r="L89" s="28"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B90" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="15">
+        <v>2000000</v>
+      </c>
+      <c r="D90" s="28">
+        <v>67.11</v>
+      </c>
+      <c r="E90" s="44">
+        <v>64</v>
+      </c>
+      <c r="F90" s="44">
+        <v>71.88</v>
+      </c>
+      <c r="G90" s="44">
+        <v>6</v>
+      </c>
+      <c r="H90" s="44">
+        <v>7.29</v>
+      </c>
+      <c r="I90" s="44">
+        <v>1.05</v>
+      </c>
+      <c r="J90" s="44">
+        <v>80</v>
+      </c>
+      <c r="K90" s="21">
+        <v>30</v>
+      </c>
+      <c r="L90" s="28">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B91" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D91" s="28"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="44"/>
+      <c r="H91" s="44"/>
+      <c r="I91" s="44"/>
+      <c r="J91" s="44"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="28"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B92" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D92" s="28"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="44"/>
+      <c r="I92" s="44"/>
+      <c r="J92" s="44"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="28"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B93" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D93" s="28"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="44"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="44"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="28"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D94" s="28"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="44"/>
+      <c r="I94" s="44"/>
+      <c r="J94" s="44"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="28"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B95" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D95" s="28"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="44"/>
+      <c r="I95" s="44"/>
+      <c r="J95" s="44"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="28"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B96" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D96" s="28"/>
+      <c r="E96" s="44"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="44"/>
+      <c r="I96" s="44"/>
+      <c r="J96" s="44"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="28"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C97" s="15">
+        <v>200000</v>
+      </c>
+      <c r="D97" s="28"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+      <c r="I97" s="44"/>
+      <c r="J97" s="44"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="28"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="15">
+        <v>20000</v>
+      </c>
+      <c r="D98" s="28"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+      <c r="I98" s="44"/>
+      <c r="J98" s="44"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="28"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B99" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="15">
+        <v>20000</v>
+      </c>
+      <c r="D99" s="28"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="44"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="44"/>
+      <c r="I99" s="44"/>
+      <c r="J99" s="44"/>
+      <c r="K99" s="22"/>
+      <c r="L99" s="29"/>
+    </row>
+    <row r="100" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="44"/>
+    </row>
+    <row r="101" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="44"/>
+      <c r="B101" s="44"/>
+      <c r="C101" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D101" s="36">
+        <f>AVERAGE(Tableau25689[Net Profit (%)])</f>
+        <v>67.11</v>
+      </c>
+      <c r="E101" s="37">
+        <f>AVERAGE(Tableau25689[Closed Trades])</f>
+        <v>64</v>
+      </c>
+      <c r="F101" s="37">
+        <f>AVERAGE(Tableau25689[% Profitable])</f>
+        <v>71.88</v>
+      </c>
+      <c r="G101" s="37">
+        <f>AVERAGE(Tableau25689[Profit Factor])</f>
+        <v>6</v>
+      </c>
+      <c r="H101" s="37">
+        <f>AVERAGE(Tableau25689[Max DrawDown])</f>
+        <v>7.29</v>
+      </c>
+      <c r="I101" s="37">
+        <f>AVERAGE(Tableau25689[Avg Trade])</f>
+        <v>1.05</v>
+      </c>
+      <c r="J101" s="37">
+        <f>AVERAGE(Tableau25689[Avg Bars in Trade])</f>
+        <v>80</v>
+      </c>
+      <c r="K101" s="37">
+        <f>AVERAGE(Tableau25689[DCA blocked (J)])</f>
+        <v>30</v>
+      </c>
+      <c r="L101" s="38">
+        <f>AVERAGE(Tableau25689[[Blocked today ]])</f>
+        <v>-2</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B87:M87"/>
     <mergeCell ref="A71:L71"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="H38:K38"/>
@@ -4084,7 +5000,7 @@
     <mergeCell ref="A55:L55"/>
   </mergeCells>
   <conditionalFormatting sqref="D39:E39 D38 E40:G50 G39">
-    <cfRule type="dataBar" priority="78">
+    <cfRule type="dataBar" priority="89">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4098,7 +5014,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D50">
-    <cfRule type="dataBar" priority="81">
+    <cfRule type="dataBar" priority="92">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4111,8 +5027,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:I51 J40:K50 I20 K39 I53:I54 I70 I86:I1048576">
-    <cfRule type="dataBar" priority="49">
+  <conditionalFormatting sqref="I39:I51 J40:K50 I20 K39 I53:I54 I70 I86 I102:I1048576">
+    <cfRule type="dataBar" priority="60">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4126,7 +5042,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D17">
-    <cfRule type="dataBar" priority="47">
+    <cfRule type="dataBar" priority="58">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4140,7 +5056,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:K37">
-    <cfRule type="dataBar" priority="45">
+    <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4154,7 +5070,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="dataBar" priority="48">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4168,7 +5084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:L7">
-    <cfRule type="dataBar" priority="44">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4182,7 +5098,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="dataBar" priority="43">
+    <cfRule type="dataBar" priority="54">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4196,7 +5112,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="dataBar" priority="42">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4209,8 +5125,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:H51 H20 H53:H54 H70 H86:H1048576">
-    <cfRule type="dataBar" priority="91">
+  <conditionalFormatting sqref="H38:H51 H20 H53:H54 H70 H86 H102:H1048576">
+    <cfRule type="dataBar" priority="102">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4224,7 +5140,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L6 D6:E6 K8:L17 E7:E17">
-    <cfRule type="dataBar" priority="92">
+    <cfRule type="dataBar" priority="103">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4238,7 +5154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F17">
-    <cfRule type="dataBar" priority="40">
+    <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4252,7 +5168,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G17">
-    <cfRule type="dataBar" priority="39">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4266,7 +5182,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H17">
-    <cfRule type="dataBar" priority="38">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4280,7 +5196,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I17">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="48">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4294,7 +5210,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J17">
-    <cfRule type="dataBar" priority="36">
+    <cfRule type="dataBar" priority="47">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4308,7 +5224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:L23">
-    <cfRule type="dataBar" priority="33">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4322,7 +5238,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:L22 D22:E22 K24:L33 E23:E33">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4336,7 +5252,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F33">
-    <cfRule type="dataBar" priority="32">
+    <cfRule type="dataBar" priority="43">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4350,7 +5266,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:G33">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4364,7 +5280,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H33">
-    <cfRule type="dataBar" priority="30">
+    <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4378,7 +5294,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I33">
-    <cfRule type="dataBar" priority="29">
+    <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4392,7 +5308,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J33">
-    <cfRule type="dataBar" priority="28">
+    <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4406,7 +5322,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4420,7 +5336,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:L56 D56:E56 K59:L59 E57:E67 K58 K66:L67 K60:K65">
-    <cfRule type="dataBar" priority="27">
+    <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4434,7 +5350,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F67">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4448,7 +5364,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:G67">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="34">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4462,7 +5378,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56:H67">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4476,7 +5392,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:I67">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4490,7 +5406,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:J67">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4504,7 +5420,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57:L58">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4518,7 +5434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:L65">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4532,7 +5448,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57:L67">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4546,7 +5462,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73:D83">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4560,7 +5476,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4574,7 +5490,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72:L72 D72:E72 K75:L75 E73:E83 K74 K82:L83 K76:K81">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4588,7 +5504,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73:F83">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4602,7 +5518,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72:G83">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4616,7 +5532,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72:H83">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4630,7 +5546,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73:I83">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4644,7 +5560,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72:J83">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4658,7 +5574,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L73:L74">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4672,7 +5588,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L76:L81">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4686,7 +5602,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L73:L83">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4700,7 +5616,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:D67">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4714,7 +5630,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D33">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4728,7 +5644,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4742,7 +5658,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N17">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4756,7 +5672,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K17">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4769,15 +5685,170 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D89:D99">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{11EAC5BD-D7BA-48F6-8BC9-4F5FE6535784}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K89">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{32A735CF-7DDF-4269-89FA-BD3CF9E80197}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88:L88 D88:E88 K91:L91 E89:E99 K90 K98:L99 K92:K97">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{472A21A8-757B-4175-9141-AE90279683B4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F89:F99">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{45C48E24-C5BA-4C3A-9A51-6F916BCCCB04}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G88:G99">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E434C604-12A1-44C5-B874-E9998757D62F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H88:H99">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0EC8F06D-2AFA-4A50-8E4B-9746302E853C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I89:I99">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{24C1A427-ED44-40E6-BFD5-E5BE7A4E7705}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J88:J99">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{ED46F683-0C5E-4640-91AB-9ACAD711ED01}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L89:L90">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DF9BE2C0-C042-4E7D-899F-959164A8B3CE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L92:L97">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{22EB45BD-9C1F-4EB3-AE29-B813E50D58D2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L89:L99">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{841116F6-6856-4088-B068-F15E99583904}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4815,7 +5886,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I39:I51 J40:K50 I20 K39 I53:I54 I70 I86:I1048576</xm:sqref>
+          <xm:sqref>I39:I51 J40:K50 I20 K39 I53:I54 I70 I86 I102:I1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BB2EB6A5-6AB7-418B-B4EC-2CEA3A48BD81}">
@@ -4898,7 +5969,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H38:H51 H20 H53:H54 H70 H86:H1048576</xm:sqref>
+          <xm:sqref>H38:H51 H20 H53:H54 H70 H86 H102:H1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{248A10D3-B8FE-465B-83E1-C1E4AC2CCDF3}">
@@ -5375,6 +6446,139 @@
           </x14:cfRule>
           <xm:sqref>K7:K17</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{11EAC5BD-D7BA-48F6-8BC9-4F5FE6535784}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D89:D99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{32A735CF-7DDF-4269-89FA-BD3CF9E80197}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K89</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{472A21A8-757B-4175-9141-AE90279683B4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K88:L88 D88:E88 K91:L91 E89:E99 K90 K98:L99 K92:K97</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{45C48E24-C5BA-4C3A-9A51-6F916BCCCB04}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F89:F99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E434C604-12A1-44C5-B874-E9998757D62F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G88:G99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0EC8F06D-2AFA-4A50-8E4B-9746302E853C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H88:H99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{24C1A427-ED44-40E6-BFD5-E5BE7A4E7705}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I89:I99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{ED46F683-0C5E-4640-91AB-9ACAD711ED01}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J88:J99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DF9BE2C0-C042-4E7D-899F-959164A8B3CE}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L89:L90</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{22EB45BD-9C1F-4EB3-AE29-B813E50D58D2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L92:L97</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{841116F6-6856-4088-B068-F15E99583904}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L89:L99</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -5511,8 +6715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5539,44 +6743,44 @@
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="32" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="32" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="32" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="32" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="32" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="10"/>
@@ -5585,7 +6789,7 @@
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>82</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -5645,6 +6849,836 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="10"/>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="113" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="114" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="117" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="120" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="122" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H122" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="123" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="124" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="125" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="128" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H128" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="134" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="135" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="136" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="138" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="139" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="140" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="141" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="142" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="143" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="144" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="145" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
@@ -5664,15 +7698,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">

</xml_diff>